<commit_message>
Tidied up code to use panda and wrap more into functions rather than linear block of code.
However, the code breaks when scrolling down now - so that's the next thing to fix.
</commit_message>
<xml_diff>
--- a/psychopy/visual/AQ.xlsx
+++ b/psychopy/visual/AQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\psychopy\psychopy\visual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{792CF266-B9C4-40DF-9974-A5F5A614A06B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5178734-444B-4CBB-A9D7-36D48FCD9112}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BE50F44C-A788-4FF8-8131-E1E95C450F0F}"/>
   </bookViews>
@@ -739,7 +739,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>